<commit_message>
cambios de calendario y duplicar
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Liv4tS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2AACE5-380D-48FC-AF24-DCE0F17E3556}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E5CDC6-2FDD-4AC8-96E4-3F1239062C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3AEA8727-4B9C-4FBD-83C6-FB813F5CA08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -757,7 +757,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,12 +772,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF22AA44"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -807,6 +801,17 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -897,48 +902,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1256,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227C099-620A-4015-B1E4-E69008B608D1}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,61 +1277,61 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1075655723</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>3153342257</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
@@ -1336,28 +1342,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>52776839</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>3125299686</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
@@ -1368,28 +1374,28 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>29111608</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>3165201327</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
@@ -1400,28 +1406,28 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>52117279</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
@@ -1432,28 +1438,28 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>1018441190</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>3103292167</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
@@ -1464,28 +1470,28 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>1013611823</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>3144626641</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I7" t="s">
@@ -1496,28 +1502,28 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>1020794049</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>3115389653</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>46</v>
       </c>
       <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I8" t="s">
@@ -1528,28 +1534,28 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>52181568</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>3118767684</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I9" t="s">
@@ -1560,28 +1566,28 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>1020741469</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>3178158654</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>56</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I10" t="s">
@@ -1592,28 +1598,28 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>52500643</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>3185630513</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>61</v>
       </c>
       <c r="G11" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I11" t="s">
@@ -1624,28 +1630,28 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>52147818</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>3112020185</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>66</v>
       </c>
       <c r="G12" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
@@ -1656,28 +1662,28 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>1020741420</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>72</v>
       </c>
       <c r="G13" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I13" t="s">
@@ -1688,28 +1694,28 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>80779572</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>3208385730</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>77</v>
       </c>
       <c r="G14" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
@@ -1720,28 +1726,28 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>20736388</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>3057074122</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>82</v>
       </c>
       <c r="G15" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="s">
@@ -1752,28 +1758,28 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>35196562</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>3157925869</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>87</v>
       </c>
       <c r="G16" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
@@ -1784,28 +1790,28 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>1020727015</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>3142382270</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>92</v>
       </c>
       <c r="G17" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
@@ -1816,28 +1822,28 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>22461099</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>3156953093</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>97</v>
       </c>
       <c r="G18" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I18" t="s">
@@ -1848,28 +1854,28 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>51630167</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>3166335609</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>102</v>
       </c>
       <c r="G19" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
@@ -1880,28 +1886,28 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>51983756</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>3105661845</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>107</v>
       </c>
       <c r="G20" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
@@ -1912,28 +1918,28 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>1018418467</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>3105765628</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>112</v>
       </c>
       <c r="G21" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I21" t="s">
@@ -1944,28 +1950,28 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>1014230868</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>3183062026</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>117</v>
       </c>
       <c r="G22" t="s">
         <v>118</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I22" t="s">
@@ -1976,28 +1982,28 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>51890441</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>3144549960</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>122</v>
       </c>
       <c r="G23" t="s">
         <v>123</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I23" t="s">
@@ -2008,28 +2014,28 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>51958580</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>3004883909</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>127</v>
       </c>
       <c r="G24" t="s">
         <v>128</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I24" t="s">
@@ -2040,28 +2046,28 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>39790138</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>3212065371</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>132</v>
       </c>
       <c r="G25" t="s">
         <v>133</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I25" t="s">
@@ -2072,28 +2078,28 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>1010170902</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>3108687778</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>137</v>
       </c>
       <c r="G26" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I26" t="s">
@@ -2104,28 +2110,28 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>79956728</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <v>3203007099</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>142</v>
       </c>
       <c r="G27" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I27" t="s">
@@ -2136,28 +2142,28 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>79502262</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>148</v>
       </c>
       <c r="G28" t="s">
         <v>149</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I28" t="s">
@@ -2167,29 +2173,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>79288759</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>3157906404</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G29" t="s">
         <v>154</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I29" t="s">
@@ -2200,28 +2206,28 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>52418314</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="9">
         <v>3103189464</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>158</v>
       </c>
       <c r="G30" t="s">
         <v>159</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I30" t="s">
@@ -2232,28 +2238,28 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>52528637</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>3125240297</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G31" t="s">
         <v>164</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I31" t="s">
@@ -2264,28 +2270,28 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>1015411257</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>3203032188</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="9" t="s">
         <v>168</v>
       </c>
       <c r="G32" t="s">
         <v>169</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I32" t="s">
@@ -2296,28 +2302,28 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>79696962</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>3133216886</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="9" t="s">
         <v>173</v>
       </c>
       <c r="G33" t="s">
         <v>174</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I33" t="s">
@@ -2328,28 +2334,28 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>53118517</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="9">
         <v>3013494846</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>178</v>
       </c>
       <c r="G34" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I34" t="s">
@@ -2360,28 +2366,28 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>52989424</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>3108660362</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="9" t="s">
         <v>183</v>
       </c>
       <c r="G35" t="s">
         <v>184</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I35" t="s">
@@ -2392,28 +2398,28 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>52249351</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="9">
         <v>3158011371</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>188</v>
       </c>
       <c r="G36" t="s">
         <v>189</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I36" t="s">
@@ -2424,28 +2430,28 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="120.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>52316683</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="14">
         <v>3107790096</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>193</v>
       </c>
       <c r="G37" t="s">
         <v>194</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I37" t="s">
@@ -2456,28 +2462,28 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>20451043</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="14">
         <v>3178860146</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="16" t="s">
         <v>198</v>
       </c>
       <c r="G38" t="s">
         <v>199</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I38" t="s">
@@ -2488,28 +2494,28 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="14">
         <v>3168210521</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="16" t="s">
         <v>204</v>
       </c>
       <c r="G39" t="s">
         <v>205</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I39" t="s">
@@ -2520,28 +2526,28 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="14">
         <v>3155293848</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="16" t="s">
         <v>210</v>
       </c>
       <c r="G40" t="s">
         <v>211</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I40" t="s">
@@ -2552,28 +2558,28 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="21">
+      <c r="A41" s="20">
         <v>368765</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="14">
         <v>3138637802</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="21" t="s">
         <v>215</v>
       </c>
       <c r="G41" t="s">
         <v>216</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I41" t="s">
@@ -2584,28 +2590,28 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="21">
+      <c r="A42" s="20">
         <v>1072643682</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="9">
         <v>3114552675</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>220</v>
       </c>
       <c r="G42" t="s">
         <v>221</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I42" t="s">
@@ -2616,28 +2622,28 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="21">
+      <c r="A43" s="20">
         <v>80134069</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="9">
         <v>3004581229</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>225</v>
       </c>
       <c r="G43" t="s">
         <v>226</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I43" t="s">
@@ -2647,29 +2653,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="21">
+    <row r="44" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
         <v>1014245299</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="9">
         <v>3138413136</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>230</v>
       </c>
       <c r="G44" t="s">
         <v>231</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I44" t="s">
@@ -2680,28 +2686,28 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="105.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="21">
+      <c r="A45" s="20">
         <v>1032456176</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="9">
         <v>3207689263</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>235</v>
       </c>
       <c r="G45" t="s">
         <v>236</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I45" t="s">
@@ -2712,28 +2718,28 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="21">
+      <c r="A46" s="20">
         <v>51881213</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="9">
         <v>3202898381</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="9" t="s">
         <v>240</v>
       </c>
       <c r="G46" t="s">
         <v>241</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I46" t="s">

</xml_diff>